<commit_message>
Event Update and created UCDiagram
Read title
</commit_message>
<xml_diff>
--- a/EventTable.xlsx
+++ b/EventTable.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17766"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel\Documents\Classes\Software Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\onlinepoker\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="936" yWindow="0" windowWidth="19560" windowHeight="8112"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
   <si>
     <t>ID</t>
   </si>
@@ -177,6 +177,21 @@
   </si>
   <si>
     <t>Player sees a list of available games</t>
+  </si>
+  <si>
+    <t>Player wants to log in to their account</t>
+  </si>
+  <si>
+    <t>Username and Password</t>
+  </si>
+  <si>
+    <t>Player is taken to their dashboard</t>
+  </si>
+  <si>
+    <t>Player / Company that the User's bank account is from</t>
+  </si>
+  <si>
+    <t>Player / SMS Respondent</t>
   </si>
 </sst>
 </file>
@@ -543,22 +558,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="32.77734375" customWidth="1"/>
-    <col min="3" max="3" width="27.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="32.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -578,248 +593,268 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+      <c r="F3" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>1.2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="D4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+      <c r="F4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" s="4" t="s">
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="F5" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B6" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="31.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="31.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="D7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+      <c r="F7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="36.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>3.1</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B8" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="D8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F7" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="F8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B9" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C9" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D9" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="F9" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C10" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="F10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B11" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="4" t="s">
+      <c r="D11" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3">
+      <c r="F11" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
         <v>3.2</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="D12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="F12" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C13" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+      <c r="F13" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>4.0999999999999996</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C14" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="4" t="s">
+      <c r="D14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update Event Table Again
</commit_message>
<xml_diff>
--- a/EventTable.xlsx
+++ b/EventTable.xlsx
@@ -209,7 +209,7 @@
     <t>Player Creates an Account</t>
   </si>
   <si>
-    <t>Name, Username, Password, Confirmed Password Cellphone # and Email address</t>
+    <t>Name, Username, Password, Confirmed Password Cellphone #, SMS Confirmation # and Email address</t>
   </si>
 </sst>
 </file>
@@ -579,7 +579,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -611,7 +611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="73.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>

</xml_diff>